<commit_message>
Procesamiento de las palabras de los títulos realizadas
</commit_message>
<xml_diff>
--- a/noticias.xlsx
+++ b/noticias.xlsx
@@ -458,12 +458,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t xml:space="preserve">CDI unveils $920M Churchill Downs Racetrack expansion plan, to be wrapped up by 154th Kentucky Derby </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>PROJECT TO BE ROLLED OUT FROM 2025-2028</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CDI unveils $920M Churchill Downs Racetrack expansion plan, to be wrapped up by 154th Kentucky Derby </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -480,12 +480,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Court dismisses Potawatomi lawsuit against Waukegan casino plans in Illinois</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>ENDS NEARLY SIX-YEAR LEGAL DISPUTE</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Court dismisses Potawatomi lawsuit against Waukegan casino plans in Illinois</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -502,12 +502,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Bally’s Corporation reportedly exploring investment in Australia’s Star Entertainment</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>BALLY’S EXECS MEET WITH STAR OFFICIALS</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Bally’s Corporation reportedly exploring investment in Australia’s Star Entertainment</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -524,12 +524,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>EGT: "We will strive to maintain and strengthen our leading positions on a global scale by entering more markets"</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>INTERVIEW WITH NADIA POPOVA</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>EGT: "We will strive to maintain and strengthen our leading positions on a global scale by entering more markets"</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -546,12 +546,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Mohegan disputes Bain Capital’s takeover of South Korea’s Inspire resort</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>REAFFIRMS COMMITMENT TO THE PROPERTY</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Mohegan disputes Bain Capital’s takeover of South Korea’s Inspire resort</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -568,12 +568,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Soft2Bet to showcase MEGA and expanding brand portfolio at SBC Summit Rio 2025</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>STAND B960; 26-27 FEBRUARY, RIOCENTRO</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Soft2Bet to showcase MEGA and expanding brand portfolio at SBC Summit Rio 2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -590,12 +590,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>SBC announces dedicated affiliation and payment summits for its Americas event in Florida</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>MAY 13TH-15TH, FORT LAUDERDALE</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SBC announces dedicated affiliation and payment summits for its Americas event in Florida</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -612,12 +612,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Unlock data's power: The smart operator’s guide</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>UPLATFORM GUIDE</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Unlock data's power: The smart operator’s guide</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -634,12 +634,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Pragmatic Play combines fast-paced action with slow-motion replays in Immersive Roulette Deluxe</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>LATEST RELEASE</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Pragmatic Play combines fast-paced action with slow-motion replays in Immersive Roulette Deluxe</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -656,12 +656,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>EstrelaBet secures definitive license to operate in Brazil’s regulated iGaming market</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t xml:space="preserve">ONE OF THE FIRST FULLY LICENSED OPERATORS </t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>EstrelaBet secures definitive license to operate in Brazil’s regulated iGaming market</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -678,12 +678,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>JCM Global secures license from Nebraska Racing and Gaming Commission</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>NOW HOLDS 178 GAMING LICENSES</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>JCM Global secures license from Nebraska Racing and Gaming Commission</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -700,12 +700,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Alabama sports betting legislation faces uphill battle amid lack of support</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>LACKS REQUIRED VOTES</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Alabama sports betting legislation faces uphill battle amid lack of support</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -722,12 +722,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Digital sports media group North Star Network acquires iGaming affiliate Bojoko</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>DEAL FINALIZED ON FEBRUARY 14</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Digital sports media group North Star Network acquires iGaming affiliate Bojoko</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Slotegrator to showcase its turnkey online casino, other key iGaming solutions at SiGMA Eurasia 2025</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>FEBRUARY 23 TO 25, DUBAI</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Slotegrator to showcase its turnkey online casino, other key iGaming solutions at SiGMA Eurasia 2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -766,12 +766,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Play’n GO announces new Egyptian-themed slot Myth of Dead</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>5-REEL, 3-ROW GAME</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Play’n GO announces new Egyptian-themed slot Myth of Dead</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -788,12 +788,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>SPiCE South Asia 2025 to gather industry leaders at Sri Lanka in two weeks</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>MARCH 4-6</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SPiCE South Asia 2025 to gather industry leaders at Sri Lanka in two weeks</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -810,12 +810,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Iowa lawmakers propose banning cities from including casinos in urban renewal plans</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>IMPACT ON CEDAR RAPIDS CASINO UNCLEAR</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Iowa lawmakers propose banning cities from including casinos in urban renewal plans</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -832,12 +832,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>BetMGM and Borgata Hotel Casino launch Evolution’s omnichannel Dual Play Baccarat in NJ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>TO CONNECT LAND-BASED AND ONLINE</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>BetMGM and Borgata Hotel Casino launch Evolution’s omnichannel Dual Play Baccarat in NJ</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -854,12 +854,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>Aristocrat Interactive's OASIS management system gains approval for rollout in Washington State</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>FOR CLASS III OPERATIONS</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Aristocrat Interactive's OASIS management system gains approval for rollout in Washington State</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -876,12 +876,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>Alpha Affiliates to attend SiGMA Eurasia and AW Dubai events in February</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>TO DISCUSS ITS VISION AND NETWORK</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Alpha Affiliates to attend SiGMA Eurasia and AW Dubai events in February</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -898,12 +898,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Gambling.com Group posts record revenue of $35.2 million in Q4 2024</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>NET INCOME REACHED $7.8 MILLION</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Gambling.com Group posts record revenue of $35.2 million in Q4 2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -920,12 +920,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>U.S. commercial gaming revenue hits record $71.9 billion in 2024</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>UP 7.5% FROM 2023</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>U.S. commercial gaming revenue hits record $71.9 billion in 2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -942,12 +942,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>IBIA launches Payment Provider Forum to bolster Brazil’s betting market integrity</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>TACKLES FINANCIAL FRAUD IN SPORTS BETTING</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>IBIA launches Payment Provider Forum to bolster Brazil’s betting market integrity</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -964,12 +964,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>Comtrade: "The Brazilian market is crying out for experienced platform operators"</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>INTERVIEW WITH STEVEN VALENTINE, CCO</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Comtrade: "The Brazilian market is crying out for experienced platform operators"</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -986,12 +986,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>Marina Bay Sands secures record $9 billion loan for casino expansion</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>AMID POST-PANDEMIC TOURISM BOOM</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Marina Bay Sands secures record $9 billion loan for casino expansion</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1008,12 +1008,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>Hudson Yards casino faces setback as Manhattan Borough President opposes rezoning</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>CURRENTLY PROPOSED PLAN "NOT GOOD ENOUGH"</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Hudson Yards casino faces setback as Manhattan Borough President opposes rezoning</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1030,12 +1030,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Iowa: Ponca Tribe expands Prairie Flower Casino, tripling gaming positions</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>FEATURES 600 SLOT MACHINES</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Iowa: Ponca Tribe expands Prairie Flower Casino, tripling gaming positions</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1052,12 +1052,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>Brazil opens public consultation on eSports regulation to boost transparency</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>UNDER ‘BETS’ REGULATIONS</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Brazil opens public consultation on eSports regulation to boost transparency</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1074,12 +1074,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>Netherlands proposes stricter gambling regulations, expansion of regulator’s powers</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>AMID PROBLEM GAMBLING CONCERNS</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Netherlands proposes stricter gambling regulations, expansion of regulator’s powers</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1096,12 +1096,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>UK Gambling Commission warns of AML failures, rising fraud risks</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>GAPS IN CUSTOMER RISK REVIEWS</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>UK Gambling Commission warns of AML failures, rising fraud risks</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1118,12 +1118,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>Fontainebleau Las Vegas expands leadership team with two key executive appointments</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>AS CASINO ENTERS SECOND YEAR</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Fontainebleau Las Vegas expands leadership team with two key executive appointments</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1140,12 +1140,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>Responsible Online Gaming Association launches new campaign on responsible gaming for college students</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t xml:space="preserve">‘KNOW YOUR PLAY’ </t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Responsible Online Gaming Association launches new campaign on responsible gaming for college students</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Microgaming transforms into Apricot Investments: analyzing the impact of this change</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>A STRATEGIC SHIFT</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Microgaming transforms into Apricot Investments: analyzing the impact of this change</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1184,12 +1184,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>Oregon bettors wager record-breaking $8.26 million on Super Bowl LIX</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>OVER 456,000 BETS WERE PLACED</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Oregon bettors wager record-breaking $8.26 million on Super Bowl LIX</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1206,100 +1206,100 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>NET INCOME RISES TO $223.6 MILLION</t>
+          <t>Uplatform's Senior Sales Manager Maria Ism to attend SiGMA Eurasia 2025 in Dubai</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>GLPI reports $389.6 million in Q4 revenue supported by expansion and new deals</t>
+          <t>FEBRUARY 23 - 25</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/11/01/50232/1667310147-peter-carlino-chairman-ceo-gaming-leisure-properties.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2025/01/21/71715/1737466566-ice-barcelona-2025-2-21-stand-uplatform.jpg</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/21/95907-glpi-reports-3896-million-in-q4-revenue-supported-by-expansion-and-new-deals</t>
+          <t>https://www.yogonet.com/international/news/2025/02/21/95915-uplatform-39s-senior-sales-manager-maria-ism-to-attend-sigma-eurasia-2025-in-dubai</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>FEBRUARY 23 - 25</t>
+          <t>AI in responsible gambling: How technological solutions are enhancing safety and security</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Uplatform's Senior Sales Manager Maria Ism to attend SiGMA Eurasia 2025 in Dubai</t>
+          <t>SLOTEGRATOR ANALYSIS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2025/01/21/71715/1737466566-ice-barcelona-2025-2-21-stand-uplatform.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2025/02/21/72792/1740141437-slotegrator-ai-in-responsible-gambling.jpg</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/21/95915-uplatform-39s-senior-sales-manager-maria-ism-to-attend-sigma-eurasia-2025-in-dubai</t>
+          <t>https://www.yogonet.com/international/news/2025/02/21/95789-ai-in-responsible-gambling-how-technological-solutions-are-enhancing-safety-and-security</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ALLEGED BREACHES OF ANTI-MONEY LAUNDERING</t>
+          <t>GLPI reports $389.6 million in Q4 revenue supported by expansion and new deals</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Entain executives resign amid legal scrutiny by AUSTRAC over alleged compliance failures</t>
+          <t>NET INCOME RISES TO $223.6 MILLION</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/08/25/57050/1692965878-entain-generica.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/11/01/50232/1667310147-peter-carlino-chairman-ceo-gaming-leisure-properties.jpg</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/21/95791-entain-executives-resign-amid-legal-scrutiny-by-austrac-over-alleged-compliance-failures</t>
+          <t>https://www.yogonet.com/international/news/2025/02/21/95907-glpi-reports-3896-million-in-q4-revenue-supported-by-expansion-and-new-deals</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SLOTEGRATOR ANALYSIS</t>
+          <t>Entain executives resign amid legal scrutiny by AUSTRAC over alleged compliance failures</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>AI in responsible gambling: How technological solutions are enhancing safety and security</t>
+          <t>ALLEGED BREACHES OF ANTI-MONEY LAUNDERING</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2025/02/21/72792/1740141437-slotegrator-ai-in-responsible-gambling.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/08/25/57050/1692965878-entain-generica.jpg</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/21/95789-ai-in-responsible-gambling-how-technological-solutions-are-enhancing-safety-and-security</t>
+          <t>https://www.yogonet.com/international/news/2025/02/21/95791-entain-executives-resign-amid-legal-scrutiny-by-austrac-over-alleged-compliance-failures</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>Macau faces intensifying regional gaming competition and economic risks, says Chief Executive</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>SAM'S FIRST POLICY ADDRESS SOON</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Macau faces intensifying regional gaming competition and economic risks, says Chief Executive</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1316,12 +1316,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>International Entertainment to invest $25.5 million in New Coast Hotel Manila revamp</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>GAMING EXPANSION WITH 110 TABLES, 920 SLOT</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>International Entertainment to invest $25.5 million in New Coast Hotel Manila revamp</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1338,12 +1338,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>Sri Lanka increases casino fees and taxes in 2025 budget in a bid to boost state revenue</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>DOUBLES ENTRY FEE FOR CASINO PATRONS</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Sri Lanka increases casino fees and taxes in 2025 budget in a bid to boost state revenue</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1360,34 +1360,34 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>NO DISRUPTIONS TO OPERATIONS</t>
+          <t>Virginia’s casino revenue surges 36% in January, led by Caesars Virginia’s growth</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>After $275M default, Bain Capital takes control of South Korea’s INSPIRE resort</t>
+          <t>INCREASED EARNINGS AS INDUSTRY EXPANDS</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/11/24/59854/1700835795-mohegan-inspire-entertainment-resort-corea-01.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2024/12/18/71025/1734531383-caesars-virginia-apertura-06.jpg</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/18/95541-after-275m-default-bain-capital-takes-control-of-south-koreas-inspire-resort</t>
+          <t>https://www.yogonet.com/international/news/2025/02/18/95542-virginias-casino-revenue-surges-36-in-january-led-by-caesars-virginias-growth</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>Pennsylvania sets state Super Bowl betting record with $101.5 million in wagers</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>A 20.4% INCREASE FROM LAST YEAR’S HIGH</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Pennsylvania sets state Super Bowl betting record with $101.5 million in wagers</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1404,12 +1404,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>Calls for legalizing basketball betting in Hong Kong resurface amid budget discussions</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>COULD GENERATE MORE THAN $128M IN TAXES</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Calls for legalizing basketball betting in Hong Kong resurface amid budget discussions</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1426,12 +1426,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>Online sports betting authorized in Buenos Aires lottery agencies</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>CAOLAB ANNOUNCEMENT</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Online sports betting authorized in Buenos Aires lottery agencies</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1448,122 +1448,122 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CURRENTLY LIMITED TO TRIBAL LAND</t>
+          <t>Hard Rock's Unity loyalty program syncs with online casino and sportsbook</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Wisconsin Policy Forum report warns of negative side effects of sports betting expansion</t>
+          <t>COMPLEMENTING EXISTING PROGRAM</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2024/11/06/69753/1730906583-apuestas-deportivas-generica-40.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2025/01/24/72011/1737743979-hard-rock-bet-generica-02.jpg</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/10/94653-wisconsin-policy-forum-report-warns-of-negative-side-effects-of-sports-betting-expansion</t>
+          <t>https://www.yogonet.com/international/news/2025/01/27/92927-hard-rock-39s-unity-loyalty-program-syncs-with-online-casino-and-sportsbook</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ONLINE CASINO REVENUE UP 14.7%</t>
+          <t>Online gaming outpaces Atlantic City casinos' revenue for the second time in January</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Denmark’s gambling revenue rises to $1.02 billion in 2024, driven by online casino growth</t>
+          <t xml:space="preserve">AC CASINOS GENERATED $210 MILLION </t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/08/30/57186/1693401909-spillemyndigheden-danish-gambling-authority.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/11/18/50654/1668799999-vista-atlantic-city-casinos.jpg</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/17/95424-denmarks-gambling-revenue-rises-to-102-billion-in-2024-driven-by-online-casino-growth</t>
+          <t>https://www.yogonet.com/international/news/2025/02/17/95412-online-gaming-outpaces-atlantic-city-casinos-39-revenue-for-the-second-time-in-january</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t xml:space="preserve">AC CASINOS GENERATED $210 MILLION </t>
+          <t>Denmark’s gambling revenue rises to $1.02 billion in 2024, driven by online casino growth</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Online gaming outpaces Atlantic City casinos' revenue for the second time in January</t>
+          <t>ONLINE CASINO REVENUE UP 14.7%</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/11/18/50654/1668799999-vista-atlantic-city-casinos.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/08/30/57186/1693401909-spillemyndigheden-danish-gambling-authority.jpg</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/17/95412-online-gaming-outpaces-atlantic-city-casinos-39-revenue-for-the-second-time-in-january</t>
+          <t>https://www.yogonet.com/international/news/2025/02/17/95424-denmarks-gambling-revenue-rises-to-102-billion-in-2024-driven-by-online-casino-growth</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>TAX SET AT 0.3% UNTIL JUNE 30, 1% FROM JULY 1</t>
+          <t>Morgan Stanley: Philippines online gaming GGR hits $2.4 billion, outpaces land-based growth</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Peru implements gradual tax increase for online gaming and sports betting</t>
+          <t>$490 MILLION GAMING TAXES GENERATED IN Q3</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2019/07/05/26492/1625331661-apuestas-online-peru-generica.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2020/09/24/33084/1625358063-juego-online-filipinas-generica.jpg</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/01/23/92673-peru-implements-gradual-tax-increase-for-online-gaming-and-sports-betting</t>
+          <t>https://www.yogonet.com/international/news/2024/12/20/89261-morgan-stanley-philippines-online-gaming-ggr-hits-24-billion-outpaces-landbased-growth</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>PART OF A BALANCED LEISURE BUDGET</t>
+          <t>Case study: How digital natives will shape online gambling in 2025</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Report reveals gambling represents 10.69% of UK consumers’ leisure spending</t>
+          <t>ANALYSIS BY BETTING OPERATOR RIVALRY</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/09/13/57568/1694610321-tarjeta-credito-juego-apuesta-online-generica-credit-card.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2025/01/15/71516/1736961707-rivalry-chronically-online-digital-natives-gambling-trends-2025-06.jpg</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/01/10/91382-report-reveals-gambling-represents-1069-of-uk-consumers-leisure-spending</t>
+          <t>https://www.yogonet.com/international/news/2025/01/15/91933-case-study-how-digital-natives-will-shape-online-gambling-in-2025</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>Hawaii sports betting bill moves forward as casino legislation fails</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>HOUSE BILL 1308 PASSES 6-4</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Hawaii sports betting bill moves forward as casino legislation fails</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1580,78 +1580,78 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>$850M UPFRONT, $200M EARN-OUT</t>
+          <t>Lawmakers reintroduce bill to eliminate federal excise tax on sports betting</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Light &amp; Wonder to acquire Grover Gaming’s charitable assets in $1.05 billion deal</t>
+          <t>TO REPEAL THE 0.25% HANDLE TAX</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/05/22/54659/1684766094-light-wonder-generica.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2019/06/13/26001/1625329682-apuestas-deportivas-generica-24.jpg</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/19/95645-light-wonder-to-acquire-grover-gamings-charitable-assets-in-105-billion-deal</t>
+          <t>https://www.yogonet.com/international/news/2025/02/19/95646-lawmakers-reintroduce-bill-to-eliminate-federal-excise-tax-on-sports-betting</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TO REPEAL THE 0.25% HANDLE TAX</t>
+          <t>Wales to become first UK nation to ban greyhound racing</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Lawmakers reintroduce bill to eliminate federal excise tax on sports betting</t>
+          <t>COULD BE IMPLEMENTED BY MAY 2026</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2019/06/13/26001/1625329682-apuestas-deportivas-generica-24.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/05/03/45369/1651597368-greyhound-carrera-galgos-generica.jpg</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/19/95646-lawmakers-reintroduce-bill-to-eliminate-federal-excise-tax-on-sports-betting</t>
+          <t>https://www.yogonet.com/international/news/2025/02/19/95658-wales-to-become-first-uk-nation-to-ban-greyhound-racing</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>COULD BE IMPLEMENTED BY MAY 2026</t>
+          <t>Light &amp; Wonder to acquire Grover Gaming’s charitable assets in $1.05 billion deal</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Wales to become first UK nation to ban greyhound racing</t>
+          <t>$850M UPFRONT, $200M EARN-OUT</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/05/03/45369/1651597368-greyhound-carrera-galgos-generica.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/05/22/54659/1684766094-light-wonder-generica.jpg</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/19/95658-wales-to-become-first-uk-nation-to-ban-greyhound-racing</t>
+          <t>https://www.yogonet.com/international/news/2025/02/19/95645-light-wonder-to-acquire-grover-gamings-charitable-assets-in-105-billion-deal</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>"Argentina is a success story for BetWarrior, and we want to replicate that in Brazil and Peru"</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>LEANDRO RIVAS, BETWARRIOR'S GENERAL MANAGER</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>"Argentina is a success story for BetWarrior, and we want to replicate that in Brazil and Peru"</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1668,12 +1668,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>Victor Arias: “Personalization and interactivity will continue to be main features this year”</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>VP OF LATAM OPERATIONS AT ARRISE POWERING PRAGMATIC PLAY</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Victor Arias: “Personalization and interactivity will continue to be main features this year”</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1690,12 +1690,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>"Regulating the Game 2025 Sydney is THE event for anyone serious about shaping the future of gambling regulation"</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>INTERVIEW WITH PAUL NEWSON</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>"Regulating the Game 2025 Sydney is THE event for anyone serious about shaping the future of gambling regulation"</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1712,12 +1712,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>SUZOHAPP: "The focus for 2025 is to re-energize the company and be that partner that everyone who's worked with us knows"</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>INTERVIEW AT ICE BARCELONA 2025</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>SUZOHAPP: "The focus for 2025 is to re-energize the company and be that partner that everyone who's worked with us knows"</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1734,12 +1734,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
+          <t>The Scatters Club Streamers Awards 2025 is a week away</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
           <t>TO TAKE PLACE ON FEB.27</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>The Scatters Club Streamers Awards 2025 is a week away</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1756,12 +1756,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
+          <t>SBC Summit Rio's second edition to return next week, marking Brazil's first post-regulation event</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
           <t>25 - 27 FEBRUARY, RIOCENTRO</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>SBC Summit Rio's second edition to return next week, marking Brazil's first post-regulation event</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1778,12 +1778,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>World Series of Poker announces full schedule for 2025 summer series</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
           <t>FROM MAY 27 TO JULY 16</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>World Series of Poker announces full schedule for 2025 summer series</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1800,12 +1800,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>SBC Summit Rio to highlight Brazil's regulatory shifts through dedicated panels</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
           <t>CAN'T-MISS REGULATORY PANELS</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>SBC Summit Rio to highlight Brazil's regulatory shifts through dedicated panels</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1822,100 +1822,100 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>INCLUDING A RANKING SYSTEM</t>
+          <t>Rivalry launches "industry-first" same-game parlays for esports</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Greentube updates its mobile esports game Ski Challenge with new features</t>
+          <t>LEAGUE OF LEGENDS, COUNTER-STRIKE, DOTA 2</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/08/30/48562/1661861789-michael-bauer-greentube-ski-challenge.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/08/23/57007/1692793030-rivalry-same-game-combo-02-mobile.jpg</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2023/01/03/65572-greentube-updates-its-mobile-esports-game-ski-challenge-with-new-features</t>
+          <t>https://www.yogonet.com/international/news/2023/08/23/68445-rivalry-launches-34industryfirst-34-samegame-parlays-for-esports</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>TARGETING FURTHER GROWTH IN 2023</t>
+          <t>Rivalry releases year-end report outlining the esports betting industry in 2022</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>unikrn to launch revamped esports betting platform in Brazil and Canada</t>
+          <t>FROM MOST BET-ON TITLES TO TRENDS</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/12/01/50888/1669907813-justin-dellario-ceo-unikrn.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/12/21/51258/1671629708-rivalry-wrapped-2022.jpg</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2022/12/01/65235-unikrn-to-launch-revamped-esports-betting-platform-in-brazil-and-canada</t>
+          <t>https://www.yogonet.com/international/news/2022/12/21/65496-rivalry-releases-yearend-report-outlining-the-esports-betting-industry-in-2022</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>FOR TWO POPULAR ESPORTS EVENTS</t>
+          <t>Thunderpick and HEROIC unveil Path to the Pros Counter-Strike 2 tournament</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Rivalry allies with Low6 to create new free-to-play esports Pick'em game</t>
+          <t>FOR BOTH AMATEURS AND EXPERIENCED PLAYERS</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2022/04/28/45247/1651149566-rivalry-mobile-generica.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2024/06/19/65405/1718803886-thunderpick-heroic-path-to-the-pros-counter-strike-2-tournament.jpg</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2022/10/31/64843-rivalry-allies-with-low6-to-create-new-freetoplay-esports-pick-39em-game</t>
+          <t>https://www.yogonet.com/international/news/2024/06/19/72739-thunderpick-and-heroic-unveil-path-to-the-pros-counterstrike-2-tournament</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>TO DEVELOP A LONG-TERM STRATEGY</t>
+          <t>Las Vegas: Luxor's esports arena to retain HyperX sponsorship, naming rights</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>EU Parliament passes resolution to support video gaming, safeguard esports from illegal gambling and match-fixing</t>
+          <t>NAMING RIGHTS AGREEMENT RENEWAL</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2018/10/24/21923/1625250361-esports-generica-07.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2021/01/13/34645/1625364305-hyperx-esports-arena-las-vegas-allied-02.jpg</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2022/11/16/65058-eu-parliament-passes-resolution-to-support-video-gaming--safeguard-esports-from-illegal-gambling-and-matchfixing</t>
+          <t>https://www.yogonet.com/international/news/2023/05/09/67075-las-vegas-luxor-39s-esports-arena-to-retain-hyperx-sponsorship-naming-rights</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>Casino Estoril installs Novomatic's Novovision CMS following launch at sister casino</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
           <t>CASINO LISBOA WENT LIVE IN DECEMBER</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Casino Estoril installs Novomatic's Novovision CMS following launch at sister casino</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1932,22 +1932,22 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>APPROVED IN A 5-0 VOTE</t>
+          <t>Ransomware attack disrupts Sault Tribe's casinos in Michigan</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Las Vegas: Henderson approves 14.1-acre expansion for Inspirada Station site</t>
+          <t>STEALS 119 GB OF DATA</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2023/11/13/59564/1699881685-station-casinos-inspirada-hotel-henderson-render-01.jpg</t>
+          <t>https://imagenesyogonet.b-cdn.net/data/imagenes/2025/02/17/72613/1739799970-casino-maquina-generica.jpg</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://www.yogonet.com/international/news/2025/02/18/95420-las-vegas-henderson-approves-141acre-expansion-for-inspirada-station-site</t>
+          <t>https://www.yogonet.com/international/news/2025/02/18/95553-ransomware-attack-disrupts-sault-tribe-39s-casinos-in-michigan</t>
         </is>
       </c>
     </row>

</xml_diff>